<commit_message>
added capacity factor for Fukushima FORWARD
Former-commit-id: c2520125586ba09605c18c1e7faa39e8f0cb63f0 [formerly 9ec3f28301d4ad743e05791ac9ee82ac1aa23aa3]
Former-commit-id: 55ec31753d65fd80d06d77b39096db74629d94d1
</commit_message>
<xml_diff>
--- a/data/japan_costs/wind/wind_Akari.xlsx
+++ b/data/japan_costs/wind/wind_Akari.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="r8_2011_onshore" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="404">
   <si>
     <t>http://www.env.go.jp/earth/report/h23-03/chpt4.pdf</t>
   </si>
@@ -1386,9 +1386,6 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>http://www.hitachi.com/products/power/wind-turbine/products/htw2000_80/specification/index.html</t>
-  </si>
-  <si>
     <t>http://www.fukushima-forward.jp/english/pdf/pamphlet3.pdf</t>
   </si>
   <si>
@@ -1425,6 +1422,70 @@
     <rPh sb="2" eb="4">
       <t>ツウシン</t>
     </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*in this report, those are given as different factors. Here are definitions:</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Availability Factor and Capacity Factor</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>(availability factor) = (monthly hours in operation) / { 24 hrs * (the number of days in a month)}</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.hitachi.com/products/power/wind-turbine/products/htw2000_80/specification/index.html</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>light green graph on the right</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>blue graph on the left</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>orange graph on the right</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>avarage wind speed</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>8(5)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2MW windmill</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>(capacity factor) = (total power generated in a month [kWh/month]) / { (capacity [kW]) * 24 hrs * (the number of days in a month)}</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>10(7)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>5MW windmill</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>12(9)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>7MW windmill</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -1578,11 +1639,11 @@
       <charset val="128"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7030A0"/>
+      <color rgb="FF000000"/>
       <name val="游ゴシック"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -2506,6 +2567,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2539,28 +2621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3338,6 +3399,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>317760</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>97774</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1324429" y="12618357"/>
+          <a:ext cx="8364117" cy="5087060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>336813</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>69196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1324429" y="17834429"/>
+          <a:ext cx="8383170" cy="5058481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>103284</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>107891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1324429" y="23504071"/>
+          <a:ext cx="8811855" cy="2829320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>613076</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>31090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1324429" y="26905857"/>
+          <a:ext cx="8659433" cy="5020376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -6957,18 +7199,18 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="C80" s="81"/>
-      <c r="D80" s="89" t="s">
+      <c r="C80" s="88"/>
+      <c r="D80" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="E80" s="90"/>
-      <c r="F80" s="91" t="s">
+      <c r="E80" s="97"/>
+      <c r="F80" s="98" t="s">
         <v>242</v>
       </c>
-      <c r="G80" s="90"/>
+      <c r="G80" s="97"/>
     </row>
     <row r="81" spans="2:11" ht="18.5" thickBot="1">
-      <c r="C81" s="82"/>
+      <c r="C81" s="89"/>
       <c r="D81" s="24" t="s">
         <v>244</v>
       </c>
@@ -6989,13 +7231,13 @@
       <c r="D82" s="20">
         <v>2592</v>
       </c>
-      <c r="E82" s="85">
+      <c r="E82" s="92">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F82" s="61">
         <v>49</v>
       </c>
-      <c r="G82" s="87">
+      <c r="G82" s="94">
         <v>0.08</v>
       </c>
     </row>
@@ -7006,22 +7248,22 @@
       <c r="D83" s="22">
         <v>3290</v>
       </c>
-      <c r="E83" s="86"/>
+      <c r="E83" s="93"/>
       <c r="F83" s="62">
         <v>67</v>
       </c>
-      <c r="G83" s="88"/>
+      <c r="G83" s="95"/>
     </row>
     <row r="84" spans="2:11" ht="36">
       <c r="C84" s="65" t="s">
         <v>252</v>
       </c>
-      <c r="D84" s="83" t="s">
+      <c r="D84" s="90" t="s">
         <v>253</v>
       </c>
-      <c r="E84" s="83"/>
-      <c r="F84" s="83"/>
-      <c r="G84" s="84"/>
+      <c r="E84" s="90"/>
+      <c r="F84" s="90"/>
+      <c r="G84" s="91"/>
     </row>
     <row r="85" spans="2:11">
       <c r="C85" s="64" t="s">
@@ -7524,7 +7766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="116" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="116" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -7578,12 +7820,12 @@
         <v>42767</v>
       </c>
       <c r="C9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -7683,10 +7925,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I45"/>
+  <dimension ref="A2:F117"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -7698,13 +7940,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="29">
-      <c r="B2" s="96" t="s">
-        <v>384</v>
+      <c r="B2" s="85" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="74" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7714,7 +7956,7 @@
       <c r="B5" s="1">
         <v>43313</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="81" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7733,13 +7975,13 @@
       <c r="C8" s="78"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="C9" s="99" t="s">
-        <v>388</v>
+      <c r="C9" s="87" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="78" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -7753,21 +7995,21 @@
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="79" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D15" s="80" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="80" t="s">
         <v>362</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="D16" s="86" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>320</v>
       </c>
@@ -7775,7 +8017,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1</v>
       </c>
@@ -7786,7 +8028,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:6">
       <c r="C22" s="12" t="s">
         <v>323</v>
       </c>
@@ -7794,64 +8036,64 @@
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="C23" s="93" t="s">
+    <row r="23" spans="1:6">
+      <c r="C23" s="82" t="s">
         <v>325</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="C24" s="94"/>
+    <row r="24" spans="1:6">
+      <c r="C24" s="83"/>
       <c r="D24" s="12" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="C25" s="94"/>
+    <row r="25" spans="1:6">
+      <c r="C25" s="83"/>
       <c r="D25" s="12" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:6">
       <c r="C26" s="9"/>
       <c r="D26" s="12" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="C27" s="93" t="s">
+    <row r="27" spans="1:6">
+      <c r="C27" s="82" t="s">
         <v>330</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:6">
       <c r="C28" s="9"/>
       <c r="D28" s="12" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="C29" s="93" t="s">
+    <row r="29" spans="1:6">
+      <c r="C29" s="82" t="s">
         <v>334</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="I29" s="78" t="s">
+      <c r="F29" s="78" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:6">
       <c r="C30" s="9"/>
       <c r="D30" s="12" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:6">
       <c r="C31" s="12" t="s">
         <v>338</v>
       </c>
@@ -7859,7 +8101,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:6">
       <c r="C32" s="12" t="s">
         <v>340</v>
       </c>
@@ -7884,7 +8126,9 @@
       </c>
     </row>
     <row r="36" spans="2:6">
-      <c r="C36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>398</v>
+      </c>
       <c r="D36" s="12" t="s">
         <v>346</v>
       </c>
@@ -7981,15 +8225,15 @@
     </row>
     <row r="43" spans="2:6">
       <c r="C43" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D43" s="95">
+        <v>384</v>
+      </c>
+      <c r="D43" s="84">
         <v>41579</v>
       </c>
-      <c r="E43" s="95">
+      <c r="E43" s="84">
         <v>42767</v>
       </c>
-      <c r="F43" s="95">
+      <c r="F43" s="84">
         <v>42339</v>
       </c>
     </row>
@@ -8011,18 +8255,78 @@
       <c r="C45" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D45" s="98" t="s">
-        <v>379</v>
+      <c r="D45" s="78" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="99" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="74" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="C50" t="s">
+        <v>393</v>
+      </c>
+      <c r="D50" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="C51" t="s">
+        <v>394</v>
+      </c>
+      <c r="D51" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="C52" t="s">
+        <v>392</v>
+      </c>
+      <c r="D52" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>396</v>
+      </c>
+      <c r="C54" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3">
+      <c r="B102" t="s">
+        <v>400</v>
+      </c>
+      <c r="C102" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" t="s">
+        <v>402</v>
+      </c>
+      <c r="C117" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="I29" r:id="rId2"/>
+    <hyperlink ref="F29" r:id="rId2"/>
     <hyperlink ref="D16" r:id="rId3"/>
+    <hyperlink ref="D45" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added some reports of costs (seems no offshore data)
</commit_message>
<xml_diff>
--- a/data/japan_costs/wind/wind_Akari.xlsx
+++ b/data/japan_costs/wind/wind_Akari.xlsx
@@ -9,24 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="r8_2011_onshore" sheetId="1" r:id="rId1"/>
     <sheet name="r8_2011_offshore" sheetId="2" r:id="rId2"/>
     <sheet name="r9_2018" sheetId="3" r:id="rId3"/>
     <sheet name="r14_2018" sheetId="4" r:id="rId4"/>
-    <sheet name="others1" sheetId="6" r:id="rId5"/>
-    <sheet name="others2" sheetId="5" r:id="rId6"/>
-    <sheet name="Fukushima_FORWARD" sheetId="8" r:id="rId7"/>
-    <sheet name="NEDO" sheetId="7" r:id="rId8"/>
+    <sheet name="Fukushima_FORWARD" sheetId="8" r:id="rId5"/>
+    <sheet name="others1" sheetId="6" r:id="rId6"/>
+    <sheet name="1" sheetId="5" r:id="rId7"/>
+    <sheet name="2" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="424">
   <si>
     <t>http://www.env.go.jp/earth/report/h23-03/chpt4.pdf</t>
   </si>
@@ -1393,9 +1393,6 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>http://jwpa.jp/pdf/20170228_OffshoreWindPower_inJapan_r1.pdf</t>
-  </si>
-  <si>
     <t>Offshore Wind Power Development in Japan</t>
     <phoneticPr fontId="12"/>
   </si>
@@ -1410,9 +1407,6 @@
   <si>
     <t>*data hasn't been updated since 2015 in English site: http://www.fukushima-forward.jp/english/index.html</t>
     <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>http://www.fukushima-forward.jp/magazine/index.html</t>
   </si>
   <si>
     <t>研究通信</t>
@@ -1487,6 +1481,97 @@
   <si>
     <t>7MW windmill</t>
     <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.fukushima-forward.jp/magazine/index.html</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/committee/kenkyukai/energy_environment/furyoku/pdf/report_01_01.pdf</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.windpwr-generate.com/outline/cost.html</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>https://ecoracy.com/248.html</t>
+  </si>
+  <si>
+    <t>can't find source for these websites</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>construction costs: 220000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>(another: 268000-300000 JPY/kW)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>O&amp;M costs: 6000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>assumption of wind power costs in 2030</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>NEDO 再生可能エネルギー技術白書</t>
+    <rPh sb="5" eb="7">
+      <t>サイセイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ギジュツ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ハクショ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>https://www.nedo.go.jp/content/100544818.pdf</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://jwpa.jp/pdf/20170228_OffshoreWindPower_inJapan_r1.pdf</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.cerpo.t.u-tokyo.ac.jp/news/upload/25f4a217b6c9bd23cddb11ca10ee4e07f0281cc3.pdf</t>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.pp.u-tokyo.ac.jp/graspp-old/courses/2013/documents/graspp2013-5113090-4.pdf</t>
+  </si>
+  <si>
+    <t>福島県沖合での大規模浮体式洋上風力発電所建設 についての費用便益分析</t>
+  </si>
+  <si>
+    <t>cost-benefit analysis for fukushima project</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Business consignment costs</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/main/yosangaisan/fy2019/pr/en/shoshin_taka_20.pdf</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/main/yosan/yosan_fy2017/pr/energy/e_enecho_e_30.pdf</t>
+  </si>
+  <si>
+    <t>http://jwpa.jp/2015_pdf/88-33tokushu.pdf</t>
+  </si>
+  <si>
+    <t>洋上風力発電の現状と今後の展望</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1646,6 +1731,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2323,7 +2414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2588,6 +2679,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2621,7 +2715,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3355,63 +3455,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>65756</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>186121</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1302846" y="2758966"/>
-          <a:ext cx="3268126" cy="1795517"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>317760</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>97774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3449,14 +3500,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>336813</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>69196</xdr:rowOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>69195</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3493,14 +3544,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>103284</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>107891</xdr:rowOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>107892</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3537,13 +3588,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>613076</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>31090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3569,6 +3620,55 @@
         <a:xfrm>
           <a:off x="1324429" y="26905857"/>
           <a:ext cx="8659433" cy="5020376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>65756</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>186121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1302846" y="2758966"/>
+          <a:ext cx="3268126" cy="1795517"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6205,8 +6305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D156"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -6406,7 +6506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
@@ -6469,9 +6569,468 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F123"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="24.75" customWidth="1"/>
+    <col min="4" max="4" width="28.4140625" customWidth="1"/>
+    <col min="5" max="5" width="17.08203125" customWidth="1"/>
+    <col min="6" max="6" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="29">
+      <c r="B2" s="85" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="74" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43313</v>
+      </c>
+      <c r="C5" s="81" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" s="78" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="78"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" s="87" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="78" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="78" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="78"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2013</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="C15" s="78" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" s="78"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="C17" s="101" t="s">
+        <v>419</v>
+      </c>
+      <c r="D17" s="80"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="C18" s="102">
+        <v>2019</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>415</v>
+      </c>
+      <c r="C19" s="80">
+        <v>2017</v>
+      </c>
+      <c r="D19" s="80" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" s="100"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" s="79" t="s">
+        <v>380</v>
+      </c>
+      <c r="D21" s="80" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" s="80" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" s="86" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>320</v>
+      </c>
+      <c r="B26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>322</v>
+      </c>
+      <c r="C27" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="C28" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="C29" s="82" t="s">
+        <v>325</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="C30" s="83"/>
+      <c r="D30" s="12" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" s="83"/>
+      <c r="D31" s="12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="C32" s="9"/>
+      <c r="D32" s="12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="C33" s="82" t="s">
+        <v>330</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="C34" s="9"/>
+      <c r="D34" s="12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="C35" s="82" t="s">
+        <v>334</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="C36" s="9"/>
+      <c r="D36" s="12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="C37" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="C39" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" t="s">
+        <v>344</v>
+      </c>
+      <c r="C41" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="C42" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="C43" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="C44" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="C45" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="C46" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="C47" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="C48" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="C49" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D49" s="84">
+        <v>41579</v>
+      </c>
+      <c r="E49" s="84">
+        <v>42767</v>
+      </c>
+      <c r="F49" s="84">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="36">
+      <c r="C50" s="60" t="s">
+        <v>377</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="C51" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D51" s="78" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="88" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="74" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="C56" t="s">
+        <v>391</v>
+      </c>
+      <c r="D56" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="C57" t="s">
+        <v>392</v>
+      </c>
+      <c r="D57" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="C58" t="s">
+        <v>390</v>
+      </c>
+      <c r="D58" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" t="s">
+        <v>394</v>
+      </c>
+      <c r="C60" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
+      <c r="B108" t="s">
+        <v>398</v>
+      </c>
+      <c r="C108" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
+      <c r="B123" t="s">
+        <v>400</v>
+      </c>
+      <c r="C123" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12"/>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="F35" r:id="rId2"/>
+    <hyperlink ref="D22" r:id="rId3"/>
+    <hyperlink ref="D51" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S116"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="61" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="61" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
@@ -7199,18 +7758,18 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="C80" s="88"/>
-      <c r="D80" s="96" t="s">
+      <c r="C80" s="89"/>
+      <c r="D80" s="97" t="s">
         <v>243</v>
       </c>
-      <c r="E80" s="97"/>
-      <c r="F80" s="98" t="s">
+      <c r="E80" s="98"/>
+      <c r="F80" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="G80" s="97"/>
+      <c r="G80" s="98"/>
     </row>
     <row r="81" spans="2:11" ht="18.5" thickBot="1">
-      <c r="C81" s="89"/>
+      <c r="C81" s="90"/>
       <c r="D81" s="24" t="s">
         <v>244</v>
       </c>
@@ -7231,13 +7790,13 @@
       <c r="D82" s="20">
         <v>2592</v>
       </c>
-      <c r="E82" s="92">
+      <c r="E82" s="93">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F82" s="61">
         <v>49</v>
       </c>
-      <c r="G82" s="94">
+      <c r="G82" s="95">
         <v>0.08</v>
       </c>
     </row>
@@ -7248,22 +7807,22 @@
       <c r="D83" s="22">
         <v>3290</v>
       </c>
-      <c r="E83" s="93"/>
+      <c r="E83" s="94"/>
       <c r="F83" s="62">
         <v>67</v>
       </c>
-      <c r="G83" s="95"/>
+      <c r="G83" s="96"/>
     </row>
     <row r="84" spans="2:11" ht="36">
       <c r="C84" s="65" t="s">
         <v>252</v>
       </c>
-      <c r="D84" s="90" t="s">
+      <c r="D84" s="91" t="s">
         <v>253</v>
       </c>
-      <c r="E84" s="90"/>
-      <c r="F84" s="90"/>
-      <c r="G84" s="91"/>
+      <c r="E84" s="91"/>
+      <c r="F84" s="91"/>
+      <c r="G84" s="92"/>
     </row>
     <row r="85" spans="2:11">
       <c r="C85" s="64" t="s">
@@ -7762,7 +8321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
@@ -7793,7 +8352,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="C3" s="78" t="s">
-        <v>294</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -7820,12 +8379,12 @@
         <v>42767</v>
       </c>
       <c r="C9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="C10" t="s">
-        <v>381</v>
+      <c r="C10" s="78" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -7917,425 +8476,22 @@
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C10" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F117"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
-  <cols>
-    <col min="3" max="3" width="24.75" customWidth="1"/>
-    <col min="4" max="4" width="28.4140625" customWidth="1"/>
-    <col min="5" max="5" width="17.08203125" customWidth="1"/>
-    <col min="6" max="6" width="26.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" ht="29">
-      <c r="B2" s="85" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="74" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43313</v>
-      </c>
-      <c r="C5" s="81" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="1"/>
-      <c r="C6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="78" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="78"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="87" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="78" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" s="78"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" s="78"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" s="78"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="C15" s="79" t="s">
-        <v>380</v>
-      </c>
-      <c r="D15" s="80" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16" s="80" t="s">
-        <v>362</v>
-      </c>
-      <c r="D16" s="86" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>320</v>
-      </c>
-      <c r="B20" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>322</v>
-      </c>
-      <c r="C21" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="C22" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="C23" s="82" t="s">
-        <v>325</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="C24" s="83"/>
-      <c r="D24" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="C25" s="83"/>
-      <c r="D25" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="C26" s="9"/>
-      <c r="D26" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="C27" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="C28" s="9"/>
-      <c r="D28" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="C29" s="82" t="s">
-        <v>334</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="F29" s="78" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="C30" s="9"/>
-      <c r="D30" s="12" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="C31" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="C32" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="C33" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>344</v>
-      </c>
-      <c r="C35" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="C36" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="C37" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="C38" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="C39" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="C40" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="C41" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="C42" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="C43" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="D43" s="84">
-        <v>41579</v>
-      </c>
-      <c r="E43" s="84">
-        <v>42767</v>
-      </c>
-      <c r="F43" s="84">
-        <v>42339</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="36">
-      <c r="C44" s="60" t="s">
-        <v>377</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="C45" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D45" s="78" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="99" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="74" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="C50" t="s">
-        <v>393</v>
-      </c>
-      <c r="D50" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="C51" t="s">
-        <v>394</v>
-      </c>
-      <c r="D51" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="C52" t="s">
-        <v>392</v>
-      </c>
-      <c r="D52" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" t="s">
-        <v>396</v>
-      </c>
-      <c r="C54" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3">
-      <c r="B102" t="s">
-        <v>400</v>
-      </c>
-      <c r="C102" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3">
-      <c r="B117" t="s">
-        <v>402</v>
-      </c>
-      <c r="C117" t="s">
-        <v>403</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="12"/>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="F29" r:id="rId2"/>
-    <hyperlink ref="D16" r:id="rId3"/>
-    <hyperlink ref="D45" r:id="rId4"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D2"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -8343,20 +8499,88 @@
     <col min="1" max="1025" width="8.58203125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="2" spans="2:3">
+      <c r="C2" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="D2" s="78" t="s">
+    </row>
+    <row r="3" spans="2:3">
+      <c r="C3" s="78" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="C4" s="79" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>2013</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="41" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" s="78" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="1">
+        <v>42522</v>
+      </c>
+      <c r="C9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="C11" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="C12" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="C13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15">
+        <v>2015</v>
+      </c>
+      <c r="C15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="C16" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added investment cost and O&M cost
</commit_message>
<xml_diff>
--- a/data/japan_costs/wind/wind_Akari.xlsx
+++ b/data/japan_costs/wind/wind_Akari.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="995" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="r8_2011_onshore" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,17 @@
     <sheet name="r9_2018" sheetId="3" r:id="rId3"/>
     <sheet name="r14_2018" sheetId="4" r:id="rId4"/>
     <sheet name="Fukushima_FORWARD" sheetId="8" r:id="rId5"/>
-    <sheet name="others1" sheetId="6" r:id="rId6"/>
-    <sheet name="1" sheetId="5" r:id="rId7"/>
-    <sheet name="2" sheetId="7" r:id="rId8"/>
+    <sheet name="costs" sheetId="9" r:id="rId6"/>
+    <sheet name="others1" sheetId="6" r:id="rId7"/>
+    <sheet name="1" sheetId="5" r:id="rId8"/>
+    <sheet name="2" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="561">
   <si>
     <t>http://www.env.go.jp/earth/report/h23-03/chpt4.pdf</t>
   </si>
@@ -1409,24 +1410,10 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>研究通信</t>
-    <rPh sb="0" eb="2">
-      <t>ケンキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ツウシン</t>
-    </rPh>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
     <t>*in this report, those are given as different factors. Here are definitions:</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>Availability Factor and Capacity Factor</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
     <t>(availability factor) = (monthly hours in operation) / { 24 hrs * (the number of days in a month)}</t>
     <phoneticPr fontId="12"/>
   </si>
@@ -1496,10 +1483,6 @@
   </si>
   <si>
     <t>https://ecoracy.com/248.html</t>
-  </si>
-  <si>
-    <t>can't find source for these websites</t>
-    <phoneticPr fontId="12"/>
   </si>
   <si>
     <t>construction costs: 220000 JPY/kW</t>
@@ -1549,29 +1532,685 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
+    <t>福島県沖合での大規模浮体式洋上風力発電所建設 についての費用便益分析</t>
+  </si>
+  <si>
+    <t>cost-benefit analysis for fukushima project</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Business consignment costs</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/main/yosangaisan/fy2019/pr/en/shoshin_taka_20.pdf</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/main/yosan/yosan_fy2017/pr/energy/e_enecho_e_30.pdf</t>
+  </si>
+  <si>
+    <t>http://jwpa.jp/2015_pdf/88-33tokushu.pdf</t>
+  </si>
+  <si>
+    <t>洋上風力発電の現状と今後の展望</t>
+  </si>
+  <si>
     <t>http://www.pp.u-tokyo.ac.jp/graspp-old/courses/2013/documents/graspp2013-5113090-4.pdf</t>
-  </si>
-  <si>
-    <t>福島県沖合での大規模浮体式洋上風力発電所建設 についての費用便益分析</t>
-  </si>
-  <si>
-    <t>cost-benefit analysis for fukushima project</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>Business consignment costs</t>
-  </si>
-  <si>
-    <t>http://www.meti.go.jp/main/yosangaisan/fy2019/pr/en/shoshin_taka_20.pdf</t>
-  </si>
-  <si>
-    <t>http://www.meti.go.jp/main/yosan/yosan_fy2017/pr/energy/e_enecho_e_30.pdf</t>
-  </si>
-  <si>
-    <t>http://jwpa.jp/2015_pdf/88-33tokushu.pdf</t>
-  </si>
-  <si>
-    <t>洋上風力発電の現状と今後の展望</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>https://www.enecho.meti.go.jp/category/saving_and_new/new/information/180824a/pdf/report_2018_01.pdf</t>
+  </si>
+  <si>
+    <t>研究通信 (research report)(numbers in this report are shown in the graphs below)</t>
+    <rPh sb="0" eb="2">
+      <t>ケンキュウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ツウシン</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>洋上風力の調達価格に係る研究会　取りまとめ報告書　参考資料２</t>
+    <rPh sb="0" eb="2">
+      <t>ヨウジョウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>フウリョク</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョウタツ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>カカク</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>カカ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ケンキュウカイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>ホウコクショ</t>
+    </rPh>
+    <rPh sb="25" eb="29">
+      <t>サンコウシリョウ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/shingikai/santeii/pdf/012_s02_00.pdf</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>procurement price of offshore wind farm</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>referance</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>25(24)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>第12回 調達価格等算定委員会</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョウタツ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>カカク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>トウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>サンテイ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>イインカイ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/shingikai/santeii/012.html</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/shingikai/santeii/pdf/012_02_00.pdf</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/shingikai/santeii/pdf/012_03_00.pdf</t>
+  </si>
+  <si>
+    <t>http://www.meti.go.jp/shingikai/santeii/pdf/042_01_00.pdf</t>
+  </si>
+  <si>
+    <t>details of costs</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>investment cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>O&amp;M cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1. investifation cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2. designing cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>3. equipment cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>4. construction cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1.rent for land, etc.</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2. repariring cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>3. personnel expenses</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>4. insurance</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>5. property tax</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>6. else</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>26(25)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>investment cost is actual cost, but O&amp;M cost is assumpton for its first year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>固定価格買い取り制度</t>
+    <rPh sb="0" eb="2">
+      <t>コテイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カカク</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セイド</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>https://www.fit-portal.go.jp/PublicInfoSummary</t>
+  </si>
+  <si>
+    <t>choshi coast (Chiba)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>investment cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1.39 million JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2400 kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>operation period</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1/29/2013-10/17/2013</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity factor </t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>produced power</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>4474306 kWh</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>71000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>68000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>448000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>802000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>37000 JPY/kW/year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*O&amp;M cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*assume 5 people operate and meintain 1 windmill</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>28(27)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Kitakyushu coast (Fukuoka)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1980 kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>6/24/2013-10/17/2013</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1053720 kWh</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>3.35 billion JPY</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3.04 billion </t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1.539 million JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>662000 JPY/kW/year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>22000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>448000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>23000JPY</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>availability factor</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>30(29)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>31(30)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*assume 8 people operate and meintain 1 windmill</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>other details of this experimental study</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>distance from coast</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>3.1km</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>sea deapth</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>11.9m</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>average wind speed</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>7.4 m/s</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>foundation</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>gravity type</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>offshore cable</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>22 kV</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>year for construction</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2 years (including 1 year of postponement due to earthquake)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>31(30)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1.4 km</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>14.0m</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>6.9m/s</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>jacket-gravity hybrid type</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>6.6 kV</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>1year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>offshore investment cost!!!</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>風力発電・地熱発電・中小水力発電について</t>
+    <rPh sb="0" eb="2">
+      <t>フウリョク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ハツデン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チネツ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ハツデン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>チュウショウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>スイリョク</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ハツデン</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>About wind power system, geothermal power system, and small/medium class hydroelectric power system</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>onshore investment cost and O&amp;M cost!!!</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>23(22)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the average is 354000 JPY/kW, the median is 335000 JPY/kW</t>
+  </si>
+  <si>
+    <t>capacity of 20kW and more (86 cases)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity of 7500kW and more (34 cases)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the median is 296000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the unit of y-axis is [10000JPY/kW]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the blue line is assumed investment cost in 2020 (282000 JPY/kW)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>26(25)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the average is 164000 JPY/kW/year, the median is 135000 JPY/kW/year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the median is 111000 JPY/kW/year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>from this data, they assume O&amp;M cost of the procurement cost in 2020 will be 93000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>from this data, they assume the investment cost of the procurement cost in 2020 will be 282000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the unit of y-axis is [10000JPY/kW/year]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the blue line is assumed O&amp;M cost in 2020 (93000 JPY/kW)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>27(26)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>稼働率</t>
+    <rPh sb="0" eb="2">
+      <t>カドウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>設備利用率</t>
+    <rPh sb="0" eb="2">
+      <t>セツビ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>リヨウリツ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>onshore: capacity factor (20kW and more)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>overall</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2001-2005</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2006-2010</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>installed in -2000</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2011-</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>assumption in 2020</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2017/6-2018/5</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity factor (median) [%]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2016/6-2017/5</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2015/6-2016/6</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2014/10-2015/9</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>can't find source of these websites</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>28(27)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>onshore: O&amp;M cost vs capacity (20kW and more)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>onshore: capacity vs investment cost (after FIT)(20kW and more)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>investment cost (599 cases)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the average is 139000 JPY/kW, the median is 133000 JPY/kW</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>25.6 (average of the last 3 years)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>O&amp;M cost (135 cases)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the average is 25000 JPY/kW/year, the median is 20000 JPY/kW/year</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity factor</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the average is 11.1%, the median is 10.0%</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>onshore: investment cost, O&amp;M cost, and capacity factor (less than 20kW)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the graph in the left</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the graph in the middle</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the graph in the right</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the unit of y-axis is [10000JPY/kW/year]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the unit of y-axis is [10000JPY/kW]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>the unit of y-axis is the number of cases</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity vs investment cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity vs O&amp;M cost</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>capacity factor vs no. of cases</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>*the blue words say "the assumption by 2017", which you can probably ignore</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Here ae what it says:</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>In terms of offshore, only one investment cost data "2010000 JPY/kW" (assumtion was 565000 JPY/kW) and no O&amp;M cost are reported as periodic report.</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Availability Factor and Capacity Factor (monthly)</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>offshore: monthly availability factor and capacity factor</t>
+    <phoneticPr fontId="12"/>
   </si>
 </sst>
 </file>
@@ -1752,7 +2391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -2405,6 +3044,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2414,7 +3073,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2682,6 +3341,69 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2714,15 +3436,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3456,13 +4169,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>317760</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>97774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3500,13 +4213,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>336813</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>69195</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3544,14 +4257,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>103284</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>107892</xdr:rowOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>107891</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3588,13 +4301,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>613076</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>31090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3632,6 +4345,140 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22687</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>147272</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1949983</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>22286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="574" t="33670" r="52249" b="23681"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1336989" y="18687795"/>
+          <a:ext cx="4745586" cy="2392863"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14598</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>189769</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1751724</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>51092</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="2032" t="48634" r="52688" b="17824"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1328391" y="22816206"/>
+          <a:ext cx="4554482" cy="1897702"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>620402</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>80287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>605805</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>43794</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="4717" t="22963" r="5884" b="33692"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1277299" y="28815862"/>
+          <a:ext cx="8992184" cy="2452415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -6569,14 +7416,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F123"/>
+  <dimension ref="A2:F125"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
+    <col min="2" max="2" width="10.08203125" customWidth="1"/>
     <col min="3" max="3" width="24.75" customWidth="1"/>
     <col min="4" max="4" width="28.4140625" customWidth="1"/>
     <col min="5" max="5" width="17.08203125" customWidth="1"/>
@@ -6616,421 +7464,1313 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="C8" s="78"/>
+      <c r="C8" s="78" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9" s="87" t="s">
-        <v>385</v>
+      <c r="C9" s="104" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="C10" s="78" t="s">
-        <v>402</v>
-      </c>
+      <c r="C10" s="78"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="87" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="78" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" s="78" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" s="78"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>2013</v>
+      </c>
+      <c r="C15" s="87" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="C12" s="78"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>2013</v>
-      </c>
-      <c r="C13" s="87" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" t="s">
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="C17" s="78" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="C18" s="78"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="C19" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="D19" s="80"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" s="91">
+        <v>2019</v>
+      </c>
+      <c r="D20" s="80" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C21" s="80">
+        <v>2017</v>
+      </c>
+      <c r="D21" s="80" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="C15" s="78" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="C16" s="78"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="C17" s="101" t="s">
-        <v>419</v>
-      </c>
-      <c r="D17" s="80"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="C18" s="102">
-        <v>2019</v>
-      </c>
-      <c r="D18" s="80" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>415</v>
-      </c>
-      <c r="C19" s="80">
-        <v>2017</v>
-      </c>
-      <c r="D19" s="80" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="C20" s="100"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="C21" s="79" t="s">
+    <row r="22" spans="1:4">
+      <c r="C22" s="89"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" s="79" t="s">
         <v>380</v>
       </c>
-      <c r="D21" s="80" t="s">
+      <c r="D23" s="80" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="C22" s="80" t="s">
+    <row r="24" spans="1:4">
+      <c r="C24" s="80" t="s">
         <v>362</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D24" s="86" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>320</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
+    <row r="29" spans="1:4">
+      <c r="A29">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>322</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="C28" s="12" t="s">
+    <row r="30" spans="1:4">
+      <c r="C30" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="C29" s="82" t="s">
+    <row r="31" spans="1:4">
+      <c r="C31" s="82" t="s">
         <v>325</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="C30" s="83"/>
-      <c r="D30" s="12" t="s">
+    <row r="32" spans="1:4">
+      <c r="C32" s="83"/>
+      <c r="D32" s="12" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="C31" s="83"/>
-      <c r="D31" s="12" t="s">
+    <row r="33" spans="2:6">
+      <c r="C33" s="83"/>
+      <c r="D33" s="12" t="s">
         <v>328</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="C32" s="9"/>
-      <c r="D32" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="C33" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="C34" s="9"/>
       <c r="D34" s="12" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="C35" s="82" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="F35" s="78" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="C36" s="9"/>
       <c r="D36" s="12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="C37" s="82" t="s">
+        <v>334</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F37" s="78" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" s="9"/>
+      <c r="D38" s="12" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="C37" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="C38" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="C39" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="C40" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="C41" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="B41" t="s">
+    <row r="43" spans="2:6">
+      <c r="B43" t="s">
         <v>344</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="C42" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="C43" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="C44" s="12" t="s">
-        <v>352</v>
+        <v>394</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="C45" s="12" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="C46" s="12" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="C47" s="12" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="C48" s="12" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="C49" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="C50" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="C51" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="D49" s="84">
+      <c r="D51" s="84">
         <v>41579</v>
       </c>
-      <c r="E49" s="84">
+      <c r="E51" s="84">
         <v>42767</v>
       </c>
-      <c r="F49" s="84">
+      <c r="F51" s="84">
         <v>42339</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="36">
-      <c r="C50" s="60" t="s">
+    <row r="52" spans="2:6" ht="36">
+      <c r="C52" s="60" t="s">
         <v>377</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D52" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F52" s="12" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
-      <c r="C51" s="3" t="s">
+    <row r="53" spans="2:6">
+      <c r="C53" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D51" s="78" t="s">
+      <c r="D53" s="78" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="88" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="74" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" t="s">
+        <v>521</v>
+      </c>
+      <c r="C58" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="88" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="74" t="s">
+      <c r="D58" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
-      <c r="C56" t="s">
+    <row r="59" spans="2:6">
+      <c r="B59" t="s">
+        <v>522</v>
+      </c>
+      <c r="C59" t="s">
+        <v>390</v>
+      </c>
+      <c r="D59" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="C60" t="s">
+        <v>388</v>
+      </c>
+      <c r="D60" t="s">
         <v>391</v>
       </c>
-      <c r="D56" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6">
-      <c r="C57" t="s">
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" t="s">
         <v>392</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C62" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
+      <c r="B110" t="s">
+        <v>396</v>
+      </c>
+      <c r="C110" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
-      <c r="C58" t="s">
-        <v>390</v>
-      </c>
-      <c r="D58" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6">
-      <c r="B60" t="s">
-        <v>394</v>
-      </c>
-      <c r="C60" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3">
-      <c r="B108" t="s">
+    <row r="125" spans="2:3">
+      <c r="B125" t="s">
         <v>398</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C125" t="s">
         <v>399</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3">
-      <c r="B123" t="s">
-        <v>400</v>
-      </c>
-      <c r="C123" t="s">
-        <v>401</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="F35" r:id="rId2"/>
-    <hyperlink ref="D22" r:id="rId3"/>
-    <hyperlink ref="D51" r:id="rId4"/>
-    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="F37" r:id="rId2"/>
+    <hyperlink ref="D24" r:id="rId3"/>
+    <hyperlink ref="D53" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId5"/>
+    <hyperlink ref="C17" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G159"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" zoomScale="87" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="30.9140625" customWidth="1"/>
+    <col min="5" max="5" width="17.4140625" customWidth="1"/>
+    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41649</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" s="79" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>423</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="78" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="41" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="79" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="80" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43405</v>
+      </c>
+      <c r="C11" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="41" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" s="41"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>426</v>
+      </c>
+      <c r="B18" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="43">
+        <v>1</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" t="s">
+        <v>427</v>
+      </c>
+      <c r="C20" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" s="82"/>
+      <c r="D21" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" s="83" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" s="83"/>
+      <c r="D23" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24" s="9"/>
+      <c r="D24" s="12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="C25" s="82"/>
+      <c r="D25" s="12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="C26" s="83"/>
+      <c r="D26" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="C27" s="83" t="s">
+        <v>435</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="C28" s="83"/>
+      <c r="D28" s="12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="C29" s="83"/>
+      <c r="D29" s="12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="C30" s="9"/>
+      <c r="D30" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" t="s">
+        <v>446</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>479</v>
+      </c>
+      <c r="C33" s="109" t="s">
+        <v>450</v>
+      </c>
+      <c r="D33" s="94"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="C34" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="C35" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="C36" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="C37" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="D37" s="92">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" s="97" t="s">
+        <v>478</v>
+      </c>
+      <c r="D38" s="101">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="C39" s="83"/>
+      <c r="E39" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="C40" s="83" t="s">
+        <v>451</v>
+      </c>
+      <c r="D40" s="83" t="s">
+        <v>471</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="F40" s="93" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="C41" s="83"/>
+      <c r="D41" s="83" t="s">
+        <v>452</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="C43" s="95" t="s">
+        <v>464</v>
+      </c>
+      <c r="D43" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="E43" s="80" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="C44" s="99"/>
+      <c r="D44" s="100"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" t="s">
+        <v>479</v>
+      </c>
+      <c r="C45" t="s">
+        <v>482</v>
+      </c>
+      <c r="D45" s="80"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="C46" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="C47" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="C48" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="D48" s="103" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="C49" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="C50" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="C51" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" t="s">
+        <v>466</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" t="s">
+        <v>480</v>
+      </c>
+      <c r="C55" s="109" t="s">
+        <v>467</v>
+      </c>
+      <c r="D55" s="94"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="C56" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="C57" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="C58" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="C59" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="D59" s="92">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="C60" s="93" t="s">
+        <v>478</v>
+      </c>
+      <c r="D60" s="102">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="C62" s="83" t="s">
+        <v>451</v>
+      </c>
+      <c r="D62" s="83" t="s">
+        <v>473</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="F62" s="93" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="C63" s="83"/>
+      <c r="D63" s="83" t="s">
+        <v>472</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="C65" s="95" t="s">
+        <v>464</v>
+      </c>
+      <c r="D65" s="96" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="C66" s="80" t="s">
+        <v>481</v>
+      </c>
+      <c r="D66" s="80"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="B68" t="s">
+        <v>495</v>
+      </c>
+      <c r="C68" t="s">
+        <v>482</v>
+      </c>
+      <c r="D68" s="80"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="C69" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="C70" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="C71" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="D71" s="103" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="C72" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="C73" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="C74" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="43">
+        <v>2</v>
+      </c>
+      <c r="B78" s="43" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="B79" t="s">
+        <v>506</v>
+      </c>
+      <c r="C79" s="88" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="C80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D80" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4">
+      <c r="C81" t="s">
+        <v>509</v>
+      </c>
+      <c r="D81" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4">
+      <c r="C82" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4">
+      <c r="C95" s="41" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4">
+      <c r="C96" s="74" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
+        <v>513</v>
+      </c>
+      <c r="C98" s="88" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="C99" t="s">
+        <v>508</v>
+      </c>
+      <c r="D99" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="C100" t="s">
+        <v>509</v>
+      </c>
+      <c r="D100" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="C101" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="C112" s="41" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="C113" s="74" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" t="s">
+        <v>520</v>
+      </c>
+      <c r="C115" s="88" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="C116" s="105"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="108" t="s">
+        <v>531</v>
+      </c>
+      <c r="F116" s="108"/>
+      <c r="G116" s="22"/>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="C117" s="106"/>
+      <c r="D117" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="F117" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="G117" s="12" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="C118" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="D118" s="12">
+        <v>20.2</v>
+      </c>
+      <c r="E118" s="12">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F118" s="12">
+        <v>18.7</v>
+      </c>
+      <c r="G118" s="12">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="C119" s="67" t="s">
+        <v>527</v>
+      </c>
+      <c r="D119" s="12">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E119" s="12">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="F119" s="12">
+        <v>17.7</v>
+      </c>
+      <c r="G119" s="12">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="C120" s="67" t="s">
+        <v>525</v>
+      </c>
+      <c r="D120" s="12">
+        <v>18.8</v>
+      </c>
+      <c r="E120" s="12">
+        <v>17.3</v>
+      </c>
+      <c r="F120" s="12">
+        <v>17.3</v>
+      </c>
+      <c r="G120" s="12">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="C121" s="67" t="s">
+        <v>526</v>
+      </c>
+      <c r="D121" s="12">
+        <v>19.3</v>
+      </c>
+      <c r="E121" s="12">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F121" s="12">
+        <v>18.7</v>
+      </c>
+      <c r="G121" s="12">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="C122" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="D122" s="12">
+        <v>27.2</v>
+      </c>
+      <c r="E122" s="12">
+        <v>26.8</v>
+      </c>
+      <c r="F122" s="12">
+        <v>24.8</v>
+      </c>
+      <c r="G122" s="12">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="C123" s="107" t="s">
+        <v>529</v>
+      </c>
+      <c r="D123" s="67"/>
+      <c r="E123" s="108" t="s">
+        <v>541</v>
+      </c>
+      <c r="F123" s="108"/>
+      <c r="G123" s="22"/>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" t="s">
+        <v>536</v>
+      </c>
+      <c r="C125" s="88" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7">
+      <c r="C126" t="s">
+        <v>539</v>
+      </c>
+      <c r="D126" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7">
+      <c r="C127" t="s">
+        <v>542</v>
+      </c>
+      <c r="D127" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7">
+      <c r="C128" t="s">
+        <v>544</v>
+      </c>
+      <c r="D128" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="141" spans="3:5">
+      <c r="C141" s="41" t="s">
+        <v>547</v>
+      </c>
+      <c r="D141" s="41" t="s">
+        <v>553</v>
+      </c>
+      <c r="E141" s="41" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="142" spans="3:5">
+      <c r="C142" s="74" t="s">
+        <v>548</v>
+      </c>
+      <c r="D142" s="41" t="s">
+        <v>554</v>
+      </c>
+      <c r="E142" s="41" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="143" spans="3:5">
+      <c r="C143" s="74" t="s">
+        <v>549</v>
+      </c>
+      <c r="D143" s="41" t="s">
+        <v>555</v>
+      </c>
+      <c r="E143" s="41" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="144" spans="3:5">
+      <c r="C144" s="98" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3">
+      <c r="B146" t="s">
+        <v>479</v>
+      </c>
+      <c r="C146" s="98" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3">
+      <c r="C147" s="98" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3">
+      <c r="C148" s="98"/>
+    </row>
+    <row r="149" spans="2:3">
+      <c r="C149" s="98"/>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="C150" s="98"/>
+    </row>
+    <row r="151" spans="2:3">
+      <c r="C151" s="98"/>
+    </row>
+    <row r="152" spans="2:3">
+      <c r="C152" s="98"/>
+    </row>
+    <row r="153" spans="2:3">
+      <c r="C153" s="98"/>
+    </row>
+    <row r="154" spans="2:3">
+      <c r="C154" s="98"/>
+    </row>
+    <row r="155" spans="2:3">
+      <c r="C155" s="98"/>
+    </row>
+    <row r="156" spans="2:3">
+      <c r="C156" s="98"/>
+    </row>
+    <row r="157" spans="2:3">
+      <c r="C157" s="98"/>
+    </row>
+    <row r="158" spans="2:3">
+      <c r="C158" s="98"/>
+    </row>
+    <row r="159" spans="2:3">
+      <c r="C159" s="98"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12"/>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S116"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="61" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B20" zoomScale="61" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
@@ -7758,18 +9498,18 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="C80" s="89"/>
-      <c r="D80" s="97" t="s">
+      <c r="C80" s="110"/>
+      <c r="D80" s="118" t="s">
         <v>243</v>
       </c>
-      <c r="E80" s="98"/>
-      <c r="F80" s="99" t="s">
+      <c r="E80" s="119"/>
+      <c r="F80" s="120" t="s">
         <v>242</v>
       </c>
-      <c r="G80" s="98"/>
+      <c r="G80" s="119"/>
     </row>
     <row r="81" spans="2:11" ht="18.5" thickBot="1">
-      <c r="C81" s="90"/>
+      <c r="C81" s="111"/>
       <c r="D81" s="24" t="s">
         <v>244</v>
       </c>
@@ -7790,13 +9530,13 @@
       <c r="D82" s="20">
         <v>2592</v>
       </c>
-      <c r="E82" s="93">
+      <c r="E82" s="114">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F82" s="61">
         <v>49</v>
       </c>
-      <c r="G82" s="95">
+      <c r="G82" s="116">
         <v>0.08</v>
       </c>
     </row>
@@ -7807,22 +9547,22 @@
       <c r="D83" s="22">
         <v>3290</v>
       </c>
-      <c r="E83" s="94"/>
+      <c r="E83" s="115"/>
       <c r="F83" s="62">
         <v>67</v>
       </c>
-      <c r="G83" s="96"/>
+      <c r="G83" s="117"/>
     </row>
     <row r="84" spans="2:11" ht="36">
       <c r="C84" s="65" t="s">
         <v>252</v>
       </c>
-      <c r="D84" s="91" t="s">
+      <c r="D84" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="E84" s="91"/>
-      <c r="F84" s="91"/>
-      <c r="G84" s="92"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="113"/>
     </row>
     <row r="85" spans="2:11">
       <c r="C85" s="64" t="s">
@@ -8321,12 +10061,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A16" zoomScale="68" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -8352,7 +10092,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="C3" s="78" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8384,7 +10124,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="C10" s="78" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -8465,7 +10205,7 @@
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="C29" t="s">
+      <c r="C29" s="79" t="s">
         <v>307</v>
       </c>
     </row>
@@ -8486,12 +10226,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -8511,7 +10251,7 @@
     </row>
     <row r="4" spans="2:3">
       <c r="C4" s="79" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -8519,17 +10259,17 @@
         <v>2013</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="41" t="s">
-        <v>406</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="C8" s="78" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="2:3">
@@ -8537,27 +10277,27 @@
         <v>42522</v>
       </c>
       <c r="C9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="C10" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="C11" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="C12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="C13" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="2:3">
@@ -8565,12 +10305,25 @@
         <v>2015</v>
       </c>
       <c r="C15" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="C16" t="s">
-        <v>422</v>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="C22" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>